<commit_message>
- added full commentry on the entire code - changed button/motor_control icon - adjusted visual control parameters for move choice - adjusted freuquency of motor_rhythm during motor control
</commit_message>
<xml_diff>
--- a/main_trials_template.xlsx
+++ b/main_trials_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meine Ablage\Studium\Github\Tetris_Psychopy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F3DDD5-24C2-496E-8744-290E7ADB9268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85091CEF-6B80-4F00-BD30-306B024C48E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4210" yWindow="1640" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="816" yWindow="1104" windowWidth="24792" windowHeight="10056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -82,58 +82,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{D23FBAA9-CFDC-4F65-83C8-2CE118638C17}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri Light"/>
-            <family val="2"/>
-            <scheme val="major"/>
-          </rPr>
-          <t xml:space="preserve">Values
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri Light"/>
-            <family val="2"/>
-            <scheme val="major"/>
-          </rPr>
-          <t>Each iteration of this loop, a different one of these values will be chosen. This will be the value of the variable named above.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{E0FA9AEE-4E8F-4568-9AD5-465E1E86E34E}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri Light"/>
-            <family val="2"/>
-            <scheme val="major"/>
-          </rPr>
-          <t xml:space="preserve">Values
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri Light"/>
-            <family val="2"/>
-            <scheme val="major"/>
-          </rPr>
-          <t>Each iteration of this loop, a different one of these values will be chosen. This will be the value of the variable named above.</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -156,20 +104,20 @@
     <t>Images/eye.png</t>
   </si>
   <si>
-    <t>Images/hand.png</t>
-  </si>
-  <si>
     <t>Images/crosshair.png</t>
   </si>
   <si>
     <t>control_condition</t>
   </si>
+  <si>
+    <t>Images/button.png</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,6 +148,13 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -227,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -235,6 +190,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -561,46 +520,48 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6328125" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.6328125" style="1"/>
-    <col min="5" max="16384" width="20.6328125" style="2"/>
+    <col min="2" max="2" width="20.6640625" style="1"/>
+    <col min="5" max="16384" width="20.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C4" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -615,12 +576,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -738,15 +696,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -768,16 +736,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>